<commit_message>
2 file delete(IND and PRI) and change RCA
</commit_message>
<xml_diff>
--- a/VT_REG2_RCA_V12.xlsx
+++ b/VT_REG2_RCA_V12.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr showObjects="placeholders" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\ETSAP_DemoS_VFE\DemoS_Adv_Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\testingmodels\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BC1FBE-60DC-4519-9FCC-1EA28CF38FAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9555" yWindow="45" windowWidth="9600" windowHeight="10950" tabRatio="901"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="14400" windowHeight="10035" tabRatio="901" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EB2" sheetId="133" r:id="rId1"/>
@@ -30,17 +31,27 @@
   <definedNames>
     <definedName name="FID_1">[1]AGR_Fuels!$A$2</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Maurizio Gargiulo</author>
   </authors>
   <commentList>
-    <comment ref="C8" authorId="0" shapeId="0">
+    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -58,14 +69,14 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Gary Goldstein</author>
     <author>Amit Kanudia</author>
     <author>Maurizio Gargiulo</author>
   </authors>
   <commentList>
-    <comment ref="J3" authorId="0" shapeId="0">
+    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -179,7 +190,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O3" authorId="1" shapeId="0">
+    <comment ref="O3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -205,7 +216,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P3" authorId="2" shapeId="0">
+    <comment ref="P3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -278,7 +289,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q3" authorId="2" shapeId="0">
+    <comment ref="Q3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -331,7 +342,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R3" authorId="2" shapeId="0">
+    <comment ref="R3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
       <text>
         <r>
           <rPr>
@@ -364,7 +375,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P13" authorId="2" shapeId="0">
+    <comment ref="P13" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
       <text>
         <r>
           <rPr>
@@ -457,7 +468,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q13" authorId="1" shapeId="0">
+    <comment ref="Q13" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000007000000}">
       <text>
         <r>
           <rPr>
@@ -482,7 +493,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R13" authorId="2" shapeId="0">
+    <comment ref="R13" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0200-000008000000}">
       <text>
         <r>
           <rPr>
@@ -545,7 +556,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J14" authorId="2" shapeId="0">
+    <comment ref="J14" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0200-000009000000}">
       <text>
         <r>
           <rPr>
@@ -793,14 +804,14 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Gary Goldstein</author>
     <author>Amit Kanudia</author>
     <author>Maurizio Gargiulo</author>
   </authors>
   <commentList>
-    <comment ref="L3" authorId="0" shapeId="0">
+    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -914,7 +925,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q3" authorId="1" shapeId="0">
+    <comment ref="Q3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -940,7 +951,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R3" authorId="2" shapeId="0">
+    <comment ref="R3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
@@ -1013,7 +1024,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S3" authorId="2" shapeId="0">
+    <comment ref="S3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
       <text>
         <r>
           <rPr>
@@ -1066,7 +1077,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T3" authorId="2" shapeId="0">
+    <comment ref="T3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
       <text>
         <r>
           <rPr>
@@ -1099,7 +1110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R9" authorId="2" shapeId="0">
+    <comment ref="R9" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0300-000006000000}">
       <text>
         <r>
           <rPr>
@@ -1192,7 +1203,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S9" authorId="1" shapeId="0">
+    <comment ref="S9" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0300-000007000000}">
       <text>
         <r>
           <rPr>
@@ -1217,7 +1228,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T9" authorId="2" shapeId="0">
+    <comment ref="T9" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0300-000008000000}">
       <text>
         <r>
           <rPr>
@@ -1280,7 +1291,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L10" authorId="2" shapeId="0">
+    <comment ref="L10" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0300-000009000000}">
       <text>
         <r>
           <rPr>
@@ -1528,14 +1539,14 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Gary Goldstein</author>
     <author>Amit Kanudia</author>
     <author>Maurizio Gargiulo</author>
   </authors>
   <commentList>
-    <comment ref="J3" authorId="0" shapeId="0">
+    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -1649,7 +1660,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O3" authorId="1" shapeId="0">
+    <comment ref="O3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
       <text>
         <r>
           <rPr>
@@ -1675,7 +1686,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P3" authorId="2" shapeId="0">
+    <comment ref="P3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0400-000003000000}">
       <text>
         <r>
           <rPr>
@@ -1748,7 +1759,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q3" authorId="2" shapeId="0">
+    <comment ref="Q3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0400-000004000000}">
       <text>
         <r>
           <rPr>
@@ -1801,7 +1812,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R3" authorId="2" shapeId="0">
+    <comment ref="R3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0400-000005000000}">
       <text>
         <r>
           <rPr>
@@ -1834,7 +1845,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P13" authorId="2" shapeId="0">
+    <comment ref="P13" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0400-000006000000}">
       <text>
         <r>
           <rPr>
@@ -1927,7 +1938,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q13" authorId="1" shapeId="0">
+    <comment ref="Q13" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0400-000007000000}">
       <text>
         <r>
           <rPr>
@@ -1952,7 +1963,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R13" authorId="2" shapeId="0">
+    <comment ref="R13" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0400-000008000000}">
       <text>
         <r>
           <rPr>
@@ -2015,7 +2026,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J14" authorId="2" shapeId="0">
+    <comment ref="J14" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0400-000009000000}">
       <text>
         <r>
           <rPr>
@@ -2263,14 +2274,14 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Gary Goldstein</author>
     <author>Amit Kanudia</author>
     <author>Maurizio Gargiulo</author>
   </authors>
   <commentList>
-    <comment ref="M3" authorId="0" shapeId="0">
+    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
       <text>
         <r>
           <rPr>
@@ -2384,7 +2395,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R3" authorId="1" shapeId="0">
+    <comment ref="R3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0500-000002000000}">
       <text>
         <r>
           <rPr>
@@ -2410,7 +2421,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S3" authorId="2" shapeId="0">
+    <comment ref="S3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0500-000003000000}">
       <text>
         <r>
           <rPr>
@@ -2483,7 +2494,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T3" authorId="2" shapeId="0">
+    <comment ref="T3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0500-000004000000}">
       <text>
         <r>
           <rPr>
@@ -2536,7 +2547,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U3" authorId="2" shapeId="0">
+    <comment ref="U3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0500-000005000000}">
       <text>
         <r>
           <rPr>
@@ -2569,7 +2580,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S11" authorId="2" shapeId="0">
+    <comment ref="S11" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0500-000006000000}">
       <text>
         <r>
           <rPr>
@@ -2662,7 +2673,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T11" authorId="1" shapeId="0">
+    <comment ref="T11" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0500-000007000000}">
       <text>
         <r>
           <rPr>
@@ -2687,7 +2698,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U11" authorId="2" shapeId="0">
+    <comment ref="U11" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0500-000008000000}">
       <text>
         <r>
           <rPr>
@@ -2750,7 +2761,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M12" authorId="2" shapeId="0">
+    <comment ref="M12" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0500-000009000000}">
       <text>
         <r>
           <rPr>
@@ -2998,14 +3009,14 @@
 </file>
 
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Gary Goldstein</author>
     <author>Amit Kanudia</author>
     <author>Maurizio Gargiulo</author>
   </authors>
   <commentList>
-    <comment ref="J3" authorId="0" shapeId="0">
+    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
       <text>
         <r>
           <rPr>
@@ -3119,7 +3130,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O3" authorId="1" shapeId="0">
+    <comment ref="O3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0600-000002000000}">
       <text>
         <r>
           <rPr>
@@ -3145,7 +3156,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P3" authorId="2" shapeId="0">
+    <comment ref="P3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0600-000003000000}">
       <text>
         <r>
           <rPr>
@@ -3218,7 +3229,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q3" authorId="2" shapeId="0">
+    <comment ref="Q3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0600-000004000000}">
       <text>
         <r>
           <rPr>
@@ -3271,7 +3282,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R3" authorId="2" shapeId="0">
+    <comment ref="R3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0600-000005000000}">
       <text>
         <r>
           <rPr>
@@ -3304,7 +3315,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P13" authorId="2" shapeId="0">
+    <comment ref="P13" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0600-000006000000}">
       <text>
         <r>
           <rPr>
@@ -3397,7 +3408,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q13" authorId="1" shapeId="0">
+    <comment ref="Q13" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0600-000007000000}">
       <text>
         <r>
           <rPr>
@@ -3422,7 +3433,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R13" authorId="2" shapeId="0">
+    <comment ref="R13" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0600-000008000000}">
       <text>
         <r>
           <rPr>
@@ -3485,7 +3496,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J14" authorId="2" shapeId="0">
+    <comment ref="J14" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0600-000009000000}">
       <text>
         <r>
           <rPr>
@@ -3733,14 +3744,14 @@
 </file>
 
 <file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Gary Goldstein</author>
     <author>Amit Kanudia</author>
     <author>Maurizio Gargiulo</author>
   </authors>
   <commentList>
-    <comment ref="M3" authorId="0" shapeId="0">
+    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000001000000}">
       <text>
         <r>
           <rPr>
@@ -3854,7 +3865,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R3" authorId="1" shapeId="0">
+    <comment ref="R3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0700-000002000000}">
       <text>
         <r>
           <rPr>
@@ -3880,7 +3891,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S3" authorId="2" shapeId="0">
+    <comment ref="S3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0700-000003000000}">
       <text>
         <r>
           <rPr>
@@ -3953,7 +3964,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T3" authorId="2" shapeId="0">
+    <comment ref="T3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0700-000004000000}">
       <text>
         <r>
           <rPr>
@@ -4006,7 +4017,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U3" authorId="2" shapeId="0">
+    <comment ref="U3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0700-000005000000}">
       <text>
         <r>
           <rPr>
@@ -4039,7 +4050,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S11" authorId="2" shapeId="0">
+    <comment ref="S11" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0700-000006000000}">
       <text>
         <r>
           <rPr>
@@ -4132,7 +4143,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T11" authorId="1" shapeId="0">
+    <comment ref="T11" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0700-000007000000}">
       <text>
         <r>
           <rPr>
@@ -4157,7 +4168,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U11" authorId="2" shapeId="0">
+    <comment ref="U11" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0700-000008000000}">
       <text>
         <r>
           <rPr>
@@ -4220,7 +4231,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M12" authorId="2" shapeId="0">
+    <comment ref="M12" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0700-000009000000}">
       <text>
         <r>
           <rPr>
@@ -4983,13 +4994,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="General_)"/>
-    <numFmt numFmtId="187" formatCode="\Te\x\t"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="General_)"/>
+    <numFmt numFmtId="166" formatCode="\Te\x\t"/>
   </numFmts>
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -5019,32 +5030,6 @@
       <sz val="10"/>
       <color indexed="12"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
@@ -5531,40 +5516,40 @@
   </borders>
   <cellStyleXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="167">
@@ -5583,20 +5568,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" xfId="10" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" xfId="10" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="13" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -5605,16 +5590,16 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" xfId="10" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" xfId="10" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="26" fillId="0" borderId="0" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="5" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -5631,91 +5616,91 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="28" fillId="14" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="24" fillId="14" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="5" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="5" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="17" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" xfId="10" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" xfId="10" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="179" fontId="13" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="9" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="179" fontId="13" fillId="16" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="16" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="16" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="22" fillId="11" borderId="0" xfId="11" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="20" fillId="9" borderId="5" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="18" fillId="11" borderId="0" xfId="11" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="16" fillId="9" borderId="5" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="20" fillId="9" borderId="6" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="16" fillId="9" borderId="6" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="179" fontId="20" fillId="9" borderId="7" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="9" borderId="7" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="13" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="13" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="13" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="13" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="13" fillId="16" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="16" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="13" fillId="16" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="16" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="13" fillId="16" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="16" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="179" fontId="13" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="13" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="15" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="22" fillId="11" borderId="0" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="30" fillId="7" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="18" fillId="11" borderId="0" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="7" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -5726,15 +5711,15 @@
     <xf numFmtId="2" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="0" xfId="14" applyFill="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="17" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="18" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5746,18 +5731,18 @@
     <xf numFmtId="1" fontId="0" fillId="18" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="3"/>
-    <xf numFmtId="179" fontId="12" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="3"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="3" fillId="16" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="3" fillId="16" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -5765,69 +5750,69 @@
     <xf numFmtId="0" fontId="3" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="13" fillId="16" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="16" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="13" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="13" fillId="16" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="16" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="13" fillId="16" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="16" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="13" fillId="16" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="16" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="13" fillId="16" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="16" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="13" fillId="16" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="16" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="22" fillId="11" borderId="12" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="32" fillId="5" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="18" fillId="11" borderId="12" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="22" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="13" fillId="16" borderId="2" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="9" fillId="16" borderId="2" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="16" borderId="5" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="9" fillId="16" borderId="5" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="16" borderId="18" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="9" fillId="16" borderId="18" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="16" borderId="0" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="9" fillId="16" borderId="0" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="22" fillId="11" borderId="16" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="22" fillId="11" borderId="2" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="13" fillId="16" borderId="14" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="18" fillId="11" borderId="16" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="18" fillId="11" borderId="2" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="9" fillId="16" borderId="14" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="16" borderId="6" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="9" fillId="16" borderId="6" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="17" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="2" xfId="14" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="28" fillId="14" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="24" fillId="14" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="18" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="17" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="28" fillId="14" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="24" fillId="14" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="22" fillId="11" borderId="13" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="18" fillId="11" borderId="13" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="3" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -5837,15 +5822,15 @@
     <xf numFmtId="9" fontId="4" fillId="18" borderId="0" xfId="22" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="4" fillId="17" borderId="5" xfId="14" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="17" borderId="0" xfId="14" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="17" fillId="17" borderId="0" xfId="33" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" xfId="10"/>
-    <xf numFmtId="9" fontId="21" fillId="10" borderId="0" xfId="10" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="13" fillId="17" borderId="0" xfId="33" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="10"/>
+    <xf numFmtId="9" fontId="17" fillId="10" borderId="0" xfId="10" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5857,34 +5842,34 @@
     <xf numFmtId="0" fontId="3" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="22" fillId="11" borderId="0" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="13" fillId="16" borderId="0" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="18" fillId="11" borderId="0" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="9" fillId="16" borderId="0" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="22" fillId="11" borderId="2" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="187" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="187" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="187" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="18" fillId="11" borderId="2" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="187" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="187" fontId="25" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="21" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="187" fontId="25" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="21" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="187" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="187" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="187" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="36">
     <cellStyle name="20% - Accent5" xfId="1" builtinId="46"/>
@@ -5893,36 +5878,36 @@
     <cellStyle name="Accent1" xfId="4" builtinId="29"/>
     <cellStyle name="Accent2" xfId="5" builtinId="33"/>
     <cellStyle name="Calculation" xfId="6" builtinId="22"/>
-    <cellStyle name="Comma 2" xfId="7"/>
-    <cellStyle name="Comma 2 2" xfId="8"/>
-    <cellStyle name="Comma 2 3" xfId="9"/>
+    <cellStyle name="Comma 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Comma 2 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Comma 2 3" xfId="9" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Good" xfId="10" builtinId="26"/>
     <cellStyle name="Input" xfId="11" builtinId="20"/>
-    <cellStyle name="Migliaia_tab emissioni" xfId="12"/>
+    <cellStyle name="Migliaia_tab emissioni" xfId="12" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="Neutral" xfId="13" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="14"/>
-    <cellStyle name="Normal 2" xfId="15"/>
-    <cellStyle name="Normal 2 3" xfId="16"/>
-    <cellStyle name="Normal 4" xfId="17"/>
-    <cellStyle name="Normal 4 2" xfId="18"/>
-    <cellStyle name="Normal 8" xfId="19"/>
-    <cellStyle name="Normal 9 2" xfId="20"/>
-    <cellStyle name="Normale_B2020" xfId="21"/>
+    <cellStyle name="Normal 10" xfId="14" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Normal 2" xfId="15" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Normal 2 3" xfId="16" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Normal 4" xfId="17" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Normal 4 2" xfId="18" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Normal 8" xfId="19" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Normal 9 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Normale_B2020" xfId="21" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
     <cellStyle name="Percent" xfId="22" builtinId="5"/>
-    <cellStyle name="Percent 2" xfId="23"/>
-    <cellStyle name="Percent 3" xfId="24"/>
-    <cellStyle name="Percent 3 2" xfId="25"/>
-    <cellStyle name="Percent 3 3" xfId="26"/>
-    <cellStyle name="Percent 4" xfId="27"/>
-    <cellStyle name="Percent 4 2" xfId="28"/>
-    <cellStyle name="Percent 4 3" xfId="29"/>
-    <cellStyle name="Percent 5" xfId="30"/>
-    <cellStyle name="Percent 5 2" xfId="31"/>
-    <cellStyle name="Percent 5 3" xfId="32"/>
-    <cellStyle name="Percent 6" xfId="33"/>
-    <cellStyle name="Percent 7" xfId="34"/>
-    <cellStyle name="Standard_Sce_D_Extraction" xfId="35"/>
+    <cellStyle name="Percent 2" xfId="23" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Percent 3" xfId="24" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Percent 3 2" xfId="25" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Percent 3 3" xfId="26" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Percent 4" xfId="27" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Percent 4 2" xfId="28" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Percent 4 3" xfId="29" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Percent 5" xfId="30" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Percent 5 2" xfId="31" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Percent 5 3" xfId="32" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Percent 6" xfId="33" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Percent 7" xfId="34" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="Standard_Sce_D_Extraction" xfId="35" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -5954,7 +5939,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="61660" name="Picture 6"/>
+        <xdr:cNvPr id="61660" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000DCF00000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6022,7 +6013,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="61661" name="Picture 8"/>
+        <xdr:cNvPr id="61661" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000DDF00000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6090,7 +6087,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="61662" name="Picture 3"/>
+        <xdr:cNvPr id="61662" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000DEF00000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6158,7 +6161,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="61663" name="Picture 4"/>
+        <xdr:cNvPr id="61663" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000DFF00000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6226,7 +6235,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="61664" name="Picture 5"/>
+        <xdr:cNvPr id="61664" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000E0F00000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6294,7 +6309,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="61665" name="Picture 6"/>
+        <xdr:cNvPr id="61665" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000E1F00000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6362,7 +6383,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="61666" name="Picture 7"/>
+        <xdr:cNvPr id="61666" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000E2F00000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6430,7 +6457,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="61667" name="Picture 8"/>
+        <xdr:cNvPr id="61667" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000E3F00000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6498,7 +6531,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="61668" name="Picture 9"/>
+        <xdr:cNvPr id="61668" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000E4F00000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6566,7 +6605,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="61669" name="Picture 10"/>
+        <xdr:cNvPr id="61669" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000E5F00000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6639,7 +6684,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -6792,7 +6843,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -6969,7 +7026,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -7122,7 +7185,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -7299,7 +7368,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -7452,7 +7527,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -7629,7 +7710,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -7731,7 +7818,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -8742,14 +8835,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:AA33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AC13" sqref="AC13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10105,8 +10198,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="122">
-        <f>1-E24-E25</f>
-        <v>9.9999999999999978E-2</v>
+        <v>0.4</v>
       </c>
       <c r="F26" s="117"/>
       <c r="G26" s="122">
@@ -10235,7 +10327,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="B3:O24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10436,7 +10528,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:J5"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -10474,7 +10566,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:R41"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -11381,7 +11473,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:T29"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -12042,7 +12134,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:R42"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -13029,7 +13121,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:U42"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -13916,7 +14008,7 @@
       </c>
       <c r="E22" s="78">
         <f>'EB2'!$E$6*'EB2'!$E$26/(G22*H22)*1.01</f>
-        <v>353.84945999999997</v>
+        <v>1415.3978400000003</v>
       </c>
       <c r="F22" s="82">
         <v>1</v>
@@ -13932,7 +14024,7 @@
       </c>
       <c r="K22" s="43">
         <f t="shared" si="5"/>
-        <v>106.15483799999998</v>
+        <v>424.61935200000011</v>
       </c>
       <c r="M22" s="159"/>
       <c r="N22" s="159"/>
@@ -14304,7 +14396,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B1:R42"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -15292,7 +15384,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B1:U42"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -16565,7 +16657,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16746,7 +16838,7 @@
       </c>
       <c r="E14" s="138">
         <f>SUM(DemTechs_COM!K21:K25)</f>
-        <v>285.62865144999989</v>
+        <v>604.09316545000013</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">

</xml_diff>